<commit_message>
updates to the SPEC cohort notebooks
updates to the SPEC cohort notebooks
</commit_message>
<xml_diff>
--- a/raw_data/jarLeak/jarBottleMap.xlsx
+++ b/raw_data/jarLeak/jarBottleMap.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinerovinski/Documents/GitHub/krl_lrv_ph_temp_2021/raw_data/jarLeak/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52087F83-96CD-114E-A5E8-FDB155C750C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FC6BA0-13C8-C148-93FD-092B1AC46F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="1260" windowWidth="10000" windowHeight="10320" xr2:uid="{1D83EE67-F333-F840-8B79-A399D4F8F08F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{1D83EE67-F333-F840-8B79-A399D4F8F08F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -593,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C28DD45-5884-5146-BBCE-8F2309279A68}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>